<commit_message>
Update paths for test data.
</commit_message>
<xml_diff>
--- a/test-data/dates-data.xlsx
+++ b/test-data/dates-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/popkhadzeg/eclipse-workspace/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA296539-6986-6945-9B90-DD9162259F05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110C0DAB-F40F-E744-92B2-F4BC34ED67C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="1060" windowWidth="33600" windowHeight="19140" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19140" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_simple_dates" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>path</t>
   </si>
@@ -148,15 +148,6 @@
     <t>expectedLabel</t>
   </si>
   <si>
-    <t>espanol/cancer/sobrellevar/sentimientos/hoja-informativa-estres</t>
-  </si>
-  <si>
-    <t>10 de diciembre de 2012</t>
-  </si>
-  <si>
-    <t>2012-12-10T12:00:00Z</t>
-  </si>
-  <si>
     <t>espanol/investigacion/es-hedge-maze</t>
   </si>
   <si>
@@ -169,20 +160,26 @@
     <t>espanol/match-infantil-infografia</t>
   </si>
   <si>
-    <t>reconstruction-fact-sheet</t>
-  </si>
-  <si>
     <t>March 12, 2016</t>
   </si>
   <si>
     <t>2016-03-12T12:00:00Z</t>
+  </si>
+  <si>
+    <t>espanol/hoja-informativa-reconstruccion</t>
+  </si>
+  <si>
+    <t>12 de marzo de 2016</t>
+  </si>
+  <si>
+    <t>types/breast/reconstruction-fact-sheet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,6 +189,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,11 +222,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +545,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,23 +557,23 @@
     <col min="6" max="6" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -653,7 +659,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -665,15 +671,15 @@
         <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -685,10 +691,10 @@
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -764,7 +770,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,14 +779,14 @@
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -830,7 +836,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
@@ -841,7 +847,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
@@ -852,7 +858,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
@@ -863,7 +869,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>

</xml_diff>